<commit_message>
Keyword driven script 2
</commit_message>
<xml_diff>
--- a/src/test/resources/KW-Scripts/KWScript3.xlsx
+++ b/src/test/resources/KW-Scripts/KWScript3.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="120" windowWidth="28695" windowHeight="12525" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="120" windowWidth="28695" windowHeight="12525" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Login01" sheetId="2" r:id="rId1"/>
@@ -502,7 +502,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
@@ -666,8 +666,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>